<commit_message>
Adding Firmware file & Review log sheet
</commit_message>
<xml_diff>
--- a/Project Plan/CI List.xlsx
+++ b/Project Plan/CI List.xlsx
@@ -33,27 +33,12 @@
     <t>Fan_Controller.c</t>
   </si>
   <si>
-    <t>Risk Sheet</t>
-  </si>
-  <si>
-    <t>Estimation Sheet</t>
-  </si>
-  <si>
     <t>Estimation Sheet.xlsx</t>
   </si>
   <si>
     <t>Project Plan</t>
   </si>
   <si>
-    <t>Objectives.xlsx</t>
-  </si>
-  <si>
-    <t>Stakeholders.xlsx</t>
-  </si>
-  <si>
-    <t>Scope.xlsx</t>
-  </si>
-  <si>
     <t>Version control.xlsx</t>
   </si>
   <si>
@@ -111,13 +96,28 @@
     <t>CH_LCD_APIs.c</t>
   </si>
   <si>
-    <t>Project Schedule.xlsx</t>
-  </si>
-  <si>
     <t>CI LIST</t>
   </si>
   <si>
     <t>LCD</t>
+  </si>
+  <si>
+    <t>CI List.xlsx</t>
+  </si>
+  <si>
+    <t>Project Plan.xlsx</t>
+  </si>
+  <si>
+    <t>CRS&amp;SRS&amp;SIQ&amp;RTM</t>
+  </si>
+  <si>
+    <t>CRS&amp;SRS&amp;SIQ&amp;RTM.xlsx</t>
+  </si>
+  <si>
+    <t>Review Log</t>
+  </si>
+  <si>
+    <t>Review Log Sheet.xlsx</t>
   </si>
 </sst>
 </file>
@@ -127,7 +127,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +156,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -178,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -210,11 +203,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -229,13 +259,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -545,8 +587,8 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8:C11"/>
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,12 +600,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="A1" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
@@ -583,7 +625,7 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
@@ -597,10 +639,10 @@
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -608,7 +650,7 @@
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
       <c r="D5" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -616,7 +658,7 @@
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -624,17 +666,17 @@
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
       <c r="D7" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -642,7 +684,7 @@
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
       <c r="D9" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -650,7 +692,7 @@
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
       <c r="D10" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -658,19 +700,19 @@
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
       <c r="D11" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -678,7 +720,7 @@
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
       <c r="D13" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -686,7 +728,7 @@
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -694,17 +736,17 @@
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
       <c r="D15" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -712,7 +754,7 @@
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="5" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -720,7 +762,7 @@
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -728,74 +770,74 @@
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5" t="s">
-        <v>12</v>
+      <c r="A26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A20:A24"/>
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="C8:C11"/>

</xml_diff>